<commit_message>
Update Leave Card 5/22/2023 1:34 PM
</commit_message>
<xml_diff>
--- a/DILIDILI, AIREEN.xlsx
+++ b/DILIDILI, AIREEN.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="87">
   <si>
     <t>PERIOD</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>3/16,17,22/2023</t>
+  </si>
+  <si>
+    <t>5/25,26/2023</t>
   </si>
 </sst>
 </file>
@@ -680,17 +683,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -700,6 +700,9 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1622,14 +1625,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1640,16 +1643,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54">
+      <c r="F3" s="53">
         <v>38019</v>
       </c>
-      <c r="G3" s="50"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -1662,14 +1665,14 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -1695,18 +1698,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52" t="s">
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -7098,17 +7101,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
@@ -7144,9 +7147,9 @@
   <dimension ref="A2:K284"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A151" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A150" activePane="bottomLeft"/>
       <selection activeCell="B9" sqref="B9"/>
-      <selection pane="bottomLeft" activeCell="B168" sqref="B168"/>
+      <selection pane="bottomLeft" activeCell="D170" sqref="D170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7176,14 +7179,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -7194,16 +7197,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54">
+      <c r="F3" s="53">
         <v>38019</v>
       </c>
-      <c r="G3" s="50"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -7216,14 +7219,14 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -7249,18 +7252,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52" t="s">
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -7307,7 +7310,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>86.103999999999999</v>
+        <v>85.353999999999999</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -7317,7 +7320,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>195.167</v>
+        <v>196.417</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -10657,13 +10660,15 @@
         <v>45017</v>
       </c>
       <c r="B168" s="20"/>
-      <c r="C168" s="13"/>
+      <c r="C168" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D168" s="40"/>
       <c r="E168" s="9"/>
       <c r="F168" s="20"/>
-      <c r="G168" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G168" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H168" s="40"/>
       <c r="I168" s="9"/>
@@ -10674,9 +10679,13 @@
       <c r="A169" s="41">
         <v>45047</v>
       </c>
-      <c r="B169" s="20"/>
+      <c r="B169" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="C169" s="13"/>
-      <c r="D169" s="40"/>
+      <c r="D169" s="40">
+        <v>2</v>
+      </c>
       <c r="E169" s="9"/>
       <c r="F169" s="20"/>
       <c r="G169" s="13" t="str">
@@ -10686,7 +10695,9 @@
       <c r="H169" s="40"/>
       <c r="I169" s="9"/>
       <c r="J169" s="11"/>
-      <c r="K169" s="20"/>
+      <c r="K169" s="20" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="41">

</xml_diff>